<commit_message>
Fixed x-scales in SinglePlot. Found out that creating future.data_numpy decreases performance dramatically, although it is not used. The reasion is unknown yet.
</commit_message>
<xml_diff>
--- a/Src/Futures/Futures.xlsx
+++ b/Src/Futures/Futures.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\info\Documents\Python\Norgate\Src\Futures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E64E746F-A37D-4796-8C7B-61FA4CD0E4E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F9FDFDE-3093-4574-B186-51973D4E9938}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38790" yWindow="390" windowWidth="36315" windowHeight="20160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1020" yWindow="1275" windowWidth="36315" windowHeight="20160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Futures" sheetId="1" r:id="rId1"/>
@@ -87,6 +87,55 @@
         </r>
       </text>
     </comment>
+    <comment ref="G45" authorId="0" shapeId="0" xr:uid="{C6E6ECC8-890D-42E2-A0BF-3748DD13C0C2}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Vassil Lolov:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Multiplier IB is * 100,
+i.e. 37500</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H45" authorId="0" shapeId="0" xr:uid="{8C889937-0270-491E-B786-1531FCFAC2FB}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Vassil Lolov:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Margin IB 20 000 !!!</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="G132" authorId="0" shapeId="0" xr:uid="{7DC22382-55FC-49DD-AEA7-F128DFEC547A}">
       <text>
         <r>
@@ -140,7 +189,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1102" uniqueCount="386">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1104" uniqueCount="388">
   <si>
     <t>Currency</t>
   </si>
@@ -1096,9 +1145,6 @@
     <t>Remove from list</t>
   </si>
   <si>
-    <t>Margin 17000 USD</t>
-  </si>
-  <si>
     <t>cant find in IB, remove from list</t>
   </si>
   <si>
@@ -1298,6 +1344,71 @@
   </si>
   <si>
     <t>exchange_ib</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Multiplier IB = multiplier Norgate * 100 !, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>special trading hours</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>European trading hours? Spread 12:15 =</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 3-4 Ticks</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (ticksize=1)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Margin IB </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>$23.000</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, can't be traded!</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -2203,10 +2314,10 @@
   <dimension ref="A1:S139"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A10" sqref="A10:XFD10"/>
+      <selection pane="bottomRight" activeCell="M54" sqref="M54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2219,57 +2330,58 @@
     <col min="12" max="12" width="15.140625" customWidth="1"/>
     <col min="13" max="13" width="15.7109375" customWidth="1"/>
     <col min="14" max="14" width="26" customWidth="1"/>
+    <col min="15" max="15" width="19.42578125" customWidth="1"/>
     <col min="19" max="19" width="84.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>343</v>
+      </c>
+      <c r="B1" t="s">
         <v>344</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>345</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>346</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>347</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>348</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>349</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>350</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" s="4" t="s">
         <v>351</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>352</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>377</v>
-      </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" t="s">
         <v>353</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
+        <v>384</v>
+      </c>
+      <c r="N1" t="s">
         <v>354</v>
       </c>
-      <c r="M1" t="s">
-        <v>385</v>
-      </c>
-      <c r="N1" t="s">
-        <v>355</v>
-      </c>
       <c r="O1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="S1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
@@ -2280,7 +2392,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -2327,7 +2439,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -2363,7 +2475,7 @@
         <v>4</v>
       </c>
       <c r="S3" s="3" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
@@ -2374,7 +2486,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
@@ -2418,7 +2530,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D5" t="s">
         <v>0</v>
@@ -2462,7 +2574,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D6" t="s">
         <v>0</v>
@@ -2503,7 +2615,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D7" t="s">
         <v>0</v>
@@ -2541,7 +2653,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D8" t="s">
         <v>0</v>
@@ -2576,7 +2688,7 @@
         <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D9" t="s">
         <v>0</v>
@@ -2611,7 +2723,7 @@
         <v>20</v>
       </c>
       <c r="C10" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D10" t="s">
         <v>21</v>
@@ -2643,7 +2755,7 @@
         <v>25</v>
       </c>
       <c r="C11" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D11" t="s">
         <v>21</v>
@@ -2675,7 +2787,7 @@
         <v>27</v>
       </c>
       <c r="C12" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D12" t="s">
         <v>28</v>
@@ -2710,7 +2822,7 @@
         <v>31</v>
       </c>
       <c r="C13" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D13" t="s">
         <v>32</v>
@@ -2734,7 +2846,7 @@
         <v>1</v>
       </c>
       <c r="L13" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="M13" t="s">
         <v>4</v>
@@ -2754,7 +2866,7 @@
         <v>34</v>
       </c>
       <c r="C14" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D14" t="s">
         <v>35</v>
@@ -2792,7 +2904,7 @@
         <v>38</v>
       </c>
       <c r="C15" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D15" t="s">
         <v>39</v>
@@ -2830,7 +2942,7 @@
         <v>43</v>
       </c>
       <c r="C16" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D16" t="s">
         <v>28</v>
@@ -2874,7 +2986,7 @@
         <v>46</v>
       </c>
       <c r="C17" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D17" t="s">
         <v>47</v>
@@ -2915,7 +3027,7 @@
         <v>49</v>
       </c>
       <c r="C18" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D18" t="s">
         <v>35</v>
@@ -2953,7 +3065,7 @@
         <v>51</v>
       </c>
       <c r="C19" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D19" t="s">
         <v>35</v>
@@ -2988,7 +3100,7 @@
         <v>53</v>
       </c>
       <c r="C20" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D20" t="s">
         <v>0</v>
@@ -3026,7 +3138,7 @@
         <v>55</v>
       </c>
       <c r="C21" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D21" t="s">
         <v>56</v>
@@ -3056,7 +3168,7 @@
         <v>4</v>
       </c>
       <c r="P21" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
@@ -3067,7 +3179,7 @@
         <v>58</v>
       </c>
       <c r="C22" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D22" t="s">
         <v>56</v>
@@ -3111,7 +3223,7 @@
         <v>60</v>
       </c>
       <c r="C23" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D23" t="s">
         <v>32</v>
@@ -3155,7 +3267,7 @@
         <v>62</v>
       </c>
       <c r="C24" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D24" t="s">
         <v>39</v>
@@ -3176,13 +3288,13 @@
         <v>0.01</v>
       </c>
       <c r="L24" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="M24" t="s">
         <v>260</v>
       </c>
       <c r="P24" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
@@ -3193,7 +3305,7 @@
         <v>66</v>
       </c>
       <c r="C25" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D25" t="s">
         <v>56</v>
@@ -3234,7 +3346,7 @@
         <v>69</v>
       </c>
       <c r="C26" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D26" t="s">
         <v>56</v>
@@ -3264,13 +3376,13 @@
         <v>260</v>
       </c>
       <c r="N26" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="O26" t="s">
         <v>260</v>
       </c>
       <c r="P26" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
@@ -3281,7 +3393,7 @@
         <v>71</v>
       </c>
       <c r="C27" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D27" t="s">
         <v>56</v>
@@ -3311,7 +3423,7 @@
         <v>260</v>
       </c>
       <c r="N27" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="O27" t="s">
         <v>260</v>
@@ -3325,7 +3437,7 @@
         <v>73</v>
       </c>
       <c r="C28" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D28" t="s">
         <v>39</v>
@@ -3363,7 +3475,7 @@
         <v>75</v>
       </c>
       <c r="C29" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D29" t="s">
         <v>39</v>
@@ -3401,7 +3513,7 @@
         <v>77</v>
       </c>
       <c r="C30" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D30" t="s">
         <v>39</v>
@@ -3442,7 +3554,7 @@
         <v>79</v>
       </c>
       <c r="C31" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D31" t="s">
         <v>39</v>
@@ -3463,13 +3575,13 @@
         <v>0.02</v>
       </c>
       <c r="L31" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="M31" t="s">
         <v>260</v>
       </c>
       <c r="P31" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
@@ -3480,7 +3592,7 @@
         <v>81</v>
       </c>
       <c r="C32" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D32" t="s">
         <v>39</v>
@@ -3510,7 +3622,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>82</v>
       </c>
@@ -3518,7 +3630,7 @@
         <v>83</v>
       </c>
       <c r="C33" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D33" t="s">
         <v>56</v>
@@ -3542,16 +3654,16 @@
         <v>1</v>
       </c>
       <c r="L33" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="M33" t="s">
         <v>260</v>
       </c>
       <c r="P33" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>85</v>
       </c>
@@ -3559,7 +3671,7 @@
         <v>86</v>
       </c>
       <c r="C34" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D34" t="s">
         <v>56</v>
@@ -3589,7 +3701,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A35" s="15" t="s">
         <v>87</v>
       </c>
@@ -3597,7 +3709,7 @@
         <v>88</v>
       </c>
       <c r="C35" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D35" t="s">
         <v>28</v>
@@ -3621,10 +3733,10 @@
         <v>1</v>
       </c>
       <c r="P35" s="15" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>89</v>
       </c>
@@ -3632,7 +3744,7 @@
         <v>90</v>
       </c>
       <c r="C36" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D36" t="s">
         <v>91</v>
@@ -3668,7 +3780,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A37" s="15" t="s">
         <v>92</v>
       </c>
@@ -3676,7 +3788,7 @@
         <v>93</v>
       </c>
       <c r="C37" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D37" t="s">
         <v>56</v>
@@ -3700,16 +3812,16 @@
         <v>1</v>
       </c>
       <c r="L37" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="M37" t="s">
         <v>4</v>
       </c>
       <c r="P37" s="15" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>94</v>
       </c>
@@ -3717,7 +3829,7 @@
         <v>95</v>
       </c>
       <c r="C38" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D38" t="s">
         <v>96</v>
@@ -3744,7 +3856,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>97</v>
       </c>
@@ -3752,7 +3864,7 @@
         <v>98</v>
       </c>
       <c r="C39" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D39" t="s">
         <v>28</v>
@@ -3776,16 +3888,16 @@
         <v>1</v>
       </c>
       <c r="L39" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="M39" t="s">
         <v>314</v>
       </c>
       <c r="P39" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>100</v>
       </c>
@@ -3793,7 +3905,7 @@
         <v>101</v>
       </c>
       <c r="C40" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D40" t="s">
         <v>96</v>
@@ -3823,7 +3935,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>102</v>
       </c>
@@ -3831,7 +3943,7 @@
         <v>103</v>
       </c>
       <c r="C41" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D41" t="s">
         <v>91</v>
@@ -3867,7 +3979,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>104</v>
       </c>
@@ -3875,7 +3987,7 @@
         <v>105</v>
       </c>
       <c r="C42" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D42" t="s">
         <v>28</v>
@@ -3899,13 +4011,13 @@
         <v>104</v>
       </c>
       <c r="N42" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="O42" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>106</v>
       </c>
@@ -3913,7 +4025,7 @@
         <v>107</v>
       </c>
       <c r="C43" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D43" t="s">
         <v>56</v>
@@ -3937,16 +4049,16 @@
         <v>1</v>
       </c>
       <c r="L43" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="M43" t="s">
         <v>109</v>
       </c>
       <c r="P43" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>110</v>
       </c>
@@ -3954,7 +4066,7 @@
         <v>111</v>
       </c>
       <c r="C44" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D44" t="s">
         <v>56</v>
@@ -3987,15 +4099,15 @@
         <v>317</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A45" s="15" t="s">
         <v>112</v>
       </c>
       <c r="B45" t="s">
         <v>113</v>
       </c>
       <c r="C45" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D45" t="s">
         <v>35</v>
@@ -4006,10 +4118,10 @@
       <c r="F45" t="s">
         <v>36</v>
       </c>
-      <c r="G45">
+      <c r="G45" s="15">
         <v>375</v>
       </c>
-      <c r="H45">
+      <c r="H45" s="15">
         <v>6675</v>
       </c>
       <c r="I45" s="4">
@@ -4022,10 +4134,13 @@
         <v>263</v>
       </c>
       <c r="P45" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+        <v>387</v>
+      </c>
+      <c r="S45" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>114</v>
       </c>
@@ -4033,7 +4148,7 @@
         <v>115</v>
       </c>
       <c r="C46" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D46" t="s">
         <v>21</v>
@@ -4066,7 +4181,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>117</v>
       </c>
@@ -4074,7 +4189,7 @@
         <v>118</v>
       </c>
       <c r="C47" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D47" t="s">
         <v>56</v>
@@ -4098,10 +4213,10 @@
         <v>1</v>
       </c>
       <c r="P47" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>121</v>
       </c>
@@ -4109,7 +4224,7 @@
         <v>122</v>
       </c>
       <c r="C48" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D48" t="s">
         <v>35</v>
@@ -4144,7 +4259,7 @@
         <v>124</v>
       </c>
       <c r="C49" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D49" t="s">
         <v>35</v>
@@ -4182,7 +4297,7 @@
         <v>126</v>
       </c>
       <c r="C50" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D50" t="s">
         <v>96</v>
@@ -4220,7 +4335,7 @@
         <v>128</v>
       </c>
       <c r="C51" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D51" t="s">
         <v>47</v>
@@ -4258,7 +4373,7 @@
         <v>130</v>
       </c>
       <c r="C52" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D52" t="s">
         <v>56</v>
@@ -4282,13 +4397,13 @@
         <v>1</v>
       </c>
       <c r="L52" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="M52" t="s">
         <v>271</v>
       </c>
       <c r="P52" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.25">
@@ -4299,7 +4414,7 @@
         <v>132</v>
       </c>
       <c r="C53" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D53" t="s">
         <v>39</v>
@@ -4337,7 +4452,7 @@
         <v>134</v>
       </c>
       <c r="C54" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D54" t="s">
         <v>35</v>
@@ -4365,6 +4480,9 @@
       </c>
       <c r="M54" t="s">
         <v>289</v>
+      </c>
+      <c r="P54" t="s">
+        <v>386</v>
       </c>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.25">
@@ -4375,7 +4493,7 @@
         <v>136</v>
       </c>
       <c r="C55" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D55" t="s">
         <v>35</v>
@@ -4413,7 +4531,7 @@
         <v>138</v>
       </c>
       <c r="C56" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D56" t="s">
         <v>21</v>
@@ -4445,7 +4563,7 @@
         <v>140</v>
       </c>
       <c r="C57" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D57" t="s">
         <v>56</v>
@@ -4480,7 +4598,7 @@
         <v>142</v>
       </c>
       <c r="C58" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D58" t="s">
         <v>32</v>
@@ -4515,7 +4633,7 @@
         <v>144</v>
       </c>
       <c r="C59" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D59" t="s">
         <v>56</v>
@@ -4550,7 +4668,7 @@
         <v>146</v>
       </c>
       <c r="C60" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D60" t="s">
         <v>32</v>
@@ -4585,7 +4703,7 @@
         <v>148</v>
       </c>
       <c r="C61" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D61" t="s">
         <v>56</v>
@@ -4617,7 +4735,7 @@
         <v>150</v>
       </c>
       <c r="C62" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D62" t="s">
         <v>56</v>
@@ -4652,7 +4770,7 @@
         <v>152</v>
       </c>
       <c r="C63" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D63" t="s">
         <v>21</v>
@@ -4676,7 +4794,7 @@
         <v>1</v>
       </c>
       <c r="P63" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.25">
@@ -4687,7 +4805,7 @@
         <v>155</v>
       </c>
       <c r="C64" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D64" t="s">
         <v>56</v>
@@ -4722,7 +4840,7 @@
         <v>158</v>
       </c>
       <c r="C65" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D65" t="s">
         <v>28</v>
@@ -4752,7 +4870,7 @@
         <v>44</v>
       </c>
       <c r="N65" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="O65" t="s">
         <v>44</v>
@@ -4769,7 +4887,7 @@
         <v>160</v>
       </c>
       <c r="C66" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D66" t="s">
         <v>56</v>
@@ -4801,7 +4919,7 @@
         <v>163</v>
       </c>
       <c r="C67" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D67" t="s">
         <v>56</v>
@@ -4831,7 +4949,7 @@
         <v>4</v>
       </c>
       <c r="N67" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="O67" t="s">
         <v>4</v>
@@ -4845,7 +4963,7 @@
         <v>165</v>
       </c>
       <c r="C68" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D68" t="s">
         <v>56</v>
@@ -4889,7 +5007,7 @@
         <v>167</v>
       </c>
       <c r="C69" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D69" t="s">
         <v>35</v>
@@ -4924,7 +5042,7 @@
         <v>169</v>
       </c>
       <c r="C70" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D70" t="s">
         <v>91</v>
@@ -4959,7 +5077,7 @@
         <v>171</v>
       </c>
       <c r="C71" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D71" t="s">
         <v>91</v>
@@ -4994,7 +5112,7 @@
         <v>173</v>
       </c>
       <c r="C72" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D72" t="s">
         <v>28</v>
@@ -5021,7 +5139,7 @@
         <v>44</v>
       </c>
       <c r="N72" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="O72" t="s">
         <v>44</v>
@@ -5035,7 +5153,7 @@
         <v>175</v>
       </c>
       <c r="C73" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D73" t="s">
         <v>35</v>
@@ -5073,7 +5191,7 @@
         <v>177</v>
       </c>
       <c r="C74" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D74" t="s">
         <v>56</v>
@@ -5117,7 +5235,7 @@
         <v>179</v>
       </c>
       <c r="C75" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D75" t="s">
         <v>35</v>
@@ -5155,7 +5273,7 @@
         <v>181</v>
       </c>
       <c r="C76" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D76" t="s">
         <v>56</v>
@@ -5193,7 +5311,7 @@
         <v>184</v>
       </c>
       <c r="C77" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D77" t="s">
         <v>91</v>
@@ -5234,7 +5352,7 @@
         <v>186</v>
       </c>
       <c r="C78" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D78" t="s">
         <v>39</v>
@@ -5266,7 +5384,7 @@
         <v>188</v>
       </c>
       <c r="C79" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D79" t="s">
         <v>56</v>
@@ -5298,7 +5416,7 @@
         <v>190</v>
       </c>
       <c r="C80" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D80" t="s">
         <v>47</v>
@@ -5336,7 +5454,7 @@
         <v>192</v>
       </c>
       <c r="C81" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D81" t="s">
         <v>47</v>
@@ -5377,7 +5495,7 @@
         <v>194</v>
       </c>
       <c r="C82" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D82" t="s">
         <v>56</v>
@@ -5409,7 +5527,7 @@
         <v>197</v>
       </c>
       <c r="C83" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D83" t="s">
         <v>56</v>
@@ -5441,7 +5559,7 @@
         <v>199</v>
       </c>
       <c r="C84" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D84" t="s">
         <v>39</v>
@@ -5488,7 +5606,7 @@
         <v>201</v>
       </c>
       <c r="C85" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D85" t="s">
         <v>39</v>
@@ -5535,7 +5653,7 @@
         <v>203</v>
       </c>
       <c r="C86" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D86" t="s">
         <v>204</v>
@@ -5579,7 +5697,7 @@
         <v>207</v>
       </c>
       <c r="C87" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D87" t="s">
         <v>28</v>
@@ -5611,7 +5729,7 @@
         <v>209</v>
       </c>
       <c r="C88" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D88" t="s">
         <v>56</v>
@@ -5643,7 +5761,7 @@
         <v>211</v>
       </c>
       <c r="C89" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D89" t="s">
         <v>39</v>
@@ -5675,7 +5793,7 @@
         <v>213</v>
       </c>
       <c r="C90" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D90" t="s">
         <v>39</v>
@@ -5707,7 +5825,7 @@
         <v>215</v>
       </c>
       <c r="C91" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D91" t="s">
         <v>56</v>
@@ -5751,7 +5869,7 @@
         <v>217</v>
       </c>
       <c r="C92" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D92" t="s">
         <v>39</v>
@@ -5783,7 +5901,7 @@
         <v>219</v>
       </c>
       <c r="C93" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D93" t="s">
         <v>39</v>
@@ -5815,7 +5933,7 @@
         <v>221</v>
       </c>
       <c r="C94" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D94" t="s">
         <v>39</v>
@@ -5850,7 +5968,7 @@
         <v>223</v>
       </c>
       <c r="C95" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D95" t="s">
         <v>21</v>
@@ -5886,7 +6004,7 @@
         <v>156</v>
       </c>
       <c r="S95" s="15" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="96" spans="1:19" x14ac:dyDescent="0.25">
@@ -5897,7 +6015,7 @@
         <v>225</v>
       </c>
       <c r="C96" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D96" t="s">
         <v>39</v>
@@ -5935,7 +6053,7 @@
         <v>227</v>
       </c>
       <c r="C97" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D97" t="s">
         <v>21</v>
@@ -5973,7 +6091,7 @@
         <v>229</v>
       </c>
       <c r="C98" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D98" t="s">
         <v>21</v>
@@ -6008,7 +6126,7 @@
         <v>231</v>
       </c>
       <c r="C99" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D99" t="s">
         <v>39</v>
@@ -6046,7 +6164,7 @@
         <v>233</v>
       </c>
       <c r="C100" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D100" t="s">
         <v>21</v>
@@ -6084,7 +6202,7 @@
         <v>235</v>
       </c>
       <c r="C101" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D101" t="s">
         <v>39</v>
@@ -6122,7 +6240,7 @@
         <v>237</v>
       </c>
       <c r="C102" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D102" t="s">
         <v>21</v>
@@ -6160,7 +6278,7 @@
         <v>239</v>
       </c>
       <c r="C103" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D103" t="s">
         <v>21</v>
@@ -6204,7 +6322,7 @@
         <v>241</v>
       </c>
       <c r="C104" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D104" t="s">
         <v>39</v>
@@ -6242,7 +6360,7 @@
         <v>243</v>
       </c>
       <c r="C105" s="5" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D105" s="5" t="s">
         <v>21</v>
@@ -6279,7 +6397,7 @@
         <v>156</v>
       </c>
       <c r="S105" s="5" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="106" spans="1:19" s="8" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -6290,7 +6408,7 @@
         <v>2</v>
       </c>
       <c r="C106" s="11" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D106" t="s">
         <v>0</v>
@@ -6321,7 +6439,7 @@
         <v>6</v>
       </c>
       <c r="C107" s="11" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D107" t="s">
         <v>0</v>
@@ -6352,7 +6470,7 @@
         <v>8</v>
       </c>
       <c r="C108" s="11" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D108" t="s">
         <v>0</v>
@@ -6383,7 +6501,7 @@
         <v>10</v>
       </c>
       <c r="C109" s="11" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D109" t="s">
         <v>0</v>
@@ -6414,7 +6532,7 @@
         <v>12</v>
       </c>
       <c r="C110" s="11" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D110" t="s">
         <v>0</v>
@@ -6437,7 +6555,7 @@
       <c r="J110" s="2"/>
       <c r="K110" s="10"/>
       <c r="S110" s="12" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="111" spans="1:19" x14ac:dyDescent="0.25">
@@ -6445,10 +6563,10 @@
         <v>258</v>
       </c>
       <c r="B111" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C111" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D111" t="s">
         <v>28</v>
@@ -6470,18 +6588,18 @@
         <v>0.05</v>
       </c>
       <c r="S111" s="15" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="112" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
+        <v>321</v>
+      </c>
+      <c r="B112" t="s">
         <v>322</v>
       </c>
-      <c r="B112" t="s">
-        <v>323</v>
-      </c>
       <c r="C112" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D112" t="s">
         <v>56</v>
@@ -6504,13 +6622,13 @@
     </row>
     <row r="113" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
+        <v>323</v>
+      </c>
+      <c r="B113" t="s">
         <v>324</v>
       </c>
-      <c r="B113" t="s">
-        <v>325</v>
-      </c>
       <c r="C113" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D113" t="s">
         <v>28</v>
@@ -6533,13 +6651,13 @@
     </row>
     <row r="114" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
+        <v>325</v>
+      </c>
+      <c r="B114" t="s">
         <v>326</v>
       </c>
-      <c r="B114" t="s">
-        <v>327</v>
-      </c>
       <c r="C114" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D114" t="s">
         <v>28</v>
@@ -6562,13 +6680,13 @@
     </row>
     <row r="115" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
+        <v>327</v>
+      </c>
+      <c r="B115" t="s">
         <v>328</v>
       </c>
-      <c r="B115" t="s">
-        <v>329</v>
-      </c>
       <c r="C115" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D115" t="s">
         <v>28</v>
@@ -6594,10 +6712,10 @@
         <v>272</v>
       </c>
       <c r="B116" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C116" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D116" t="s">
         <v>39</v>
@@ -6623,10 +6741,10 @@
         <v>274</v>
       </c>
       <c r="B117" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C117" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D117" t="s">
         <v>39</v>
@@ -6652,10 +6770,10 @@
         <v>256</v>
       </c>
       <c r="B118" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C118" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D118" t="s">
         <v>28</v>
@@ -6681,10 +6799,10 @@
         <v>279</v>
       </c>
       <c r="B119" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C119" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D119" t="s">
         <v>21</v>
@@ -6706,7 +6824,7 @@
         <v>0.125</v>
       </c>
       <c r="S119" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="120" spans="1:19" x14ac:dyDescent="0.25">
@@ -6714,10 +6832,10 @@
         <v>277</v>
       </c>
       <c r="B120" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C120" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D120" t="s">
         <v>21</v>
@@ -6739,7 +6857,7 @@
         <v>0.125</v>
       </c>
       <c r="S120" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="121" spans="1:19" x14ac:dyDescent="0.25">
@@ -6750,7 +6868,7 @@
         <v>142</v>
       </c>
       <c r="C121" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D121" t="s">
         <v>32</v>
@@ -6779,7 +6897,7 @@
         <v>146</v>
       </c>
       <c r="C122" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D122" t="s">
         <v>32</v>
@@ -6805,10 +6923,10 @@
         <v>257</v>
       </c>
       <c r="B123" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C123" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D123" t="s">
         <v>91</v>
@@ -6837,7 +6955,7 @@
         <v>144</v>
       </c>
       <c r="C124" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D124" t="s">
         <v>56</v>
@@ -6866,7 +6984,7 @@
         <v>150</v>
       </c>
       <c r="C125" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D125" t="s">
         <v>56</v>
@@ -6895,7 +7013,7 @@
         <v>140</v>
       </c>
       <c r="C126" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D126" t="s">
         <v>56</v>
@@ -6921,10 +7039,10 @@
         <v>291</v>
       </c>
       <c r="B127" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C127" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D127" t="s">
         <v>204</v>
@@ -6953,7 +7071,7 @@
         <v>155</v>
       </c>
       <c r="C128" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D128" t="s">
         <v>56</v>
@@ -6979,10 +7097,10 @@
         <v>278</v>
       </c>
       <c r="B129" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C129" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D129" t="s">
         <v>21</v>
@@ -7004,18 +7122,18 @@
         <v>0.125</v>
       </c>
       <c r="S129" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="130" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
+        <v>363</v>
+      </c>
+      <c r="B130" t="s">
         <v>364</v>
       </c>
-      <c r="B130" t="s">
-        <v>365</v>
-      </c>
       <c r="C130" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D130" t="s">
         <v>56</v>
@@ -7038,13 +7156,13 @@
     </row>
     <row r="131" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B131" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C131" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D131" t="s">
         <v>56</v>
@@ -7067,13 +7185,13 @@
     </row>
     <row r="132" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B132" t="s">
         <v>83</v>
       </c>
       <c r="C132" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D132" t="s">
         <v>56</v>
@@ -7097,7 +7215,7 @@
         <v>1</v>
       </c>
       <c r="S132" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="133" spans="1:19" x14ac:dyDescent="0.25">
@@ -7108,7 +7226,7 @@
         <v>261</v>
       </c>
       <c r="C133" s="13" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D133" s="13" t="s">
         <v>56</v>
@@ -7129,7 +7247,7 @@
         <v>0.2</v>
       </c>
       <c r="S133" s="13" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="134" spans="1:19" x14ac:dyDescent="0.25">
@@ -7140,7 +7258,7 @@
         <v>264</v>
       </c>
       <c r="C134" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D134" t="s">
         <v>56</v>
@@ -7169,7 +7287,7 @@
         <v>290</v>
       </c>
       <c r="C135" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D135" t="s">
         <v>204</v>
@@ -7198,7 +7316,7 @@
         <v>294</v>
       </c>
       <c r="C136" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D136" t="s">
         <v>296</v>
@@ -7227,7 +7345,7 @@
         <v>297</v>
       </c>
       <c r="C137" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D137" t="s">
         <v>296</v>
@@ -7248,7 +7366,7 @@
         <v>1E-3</v>
       </c>
       <c r="S137" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="138" spans="1:19" x14ac:dyDescent="0.25">
@@ -7259,7 +7377,7 @@
         <v>298</v>
       </c>
       <c r="C138" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D138" t="s">
         <v>296</v>
@@ -7288,7 +7406,7 @@
         <v>299</v>
       </c>
       <c r="C139" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D139" t="s">
         <v>296</v>

</xml_diff>